<commit_message>
option to update menu
</commit_message>
<xml_diff>
--- a/data/food_options.xlsx
+++ b/data/food_options.xlsx
@@ -18,11 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -471,26 +469,23 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col width="22.83203125" bestFit="1" customWidth="1" min="1" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>breakfast_option</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>breakfast_description</t>
         </is>
@@ -616,7 +611,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -626,30 +621,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A8"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col width="33" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="37.83203125" bestFit="1" customWidth="1" min="2" max="2"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>lunch</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>lunch_description</t>
         </is>
@@ -774,8 +765,25 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>stage</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>